<commit_message>
feat: add concolic testing for text dataset
</commit_message>
<xml_diff>
--- a/neuron_coverage_cnn/figure 6.xlsx
+++ b/neuron_coverage_cnn/figure 6.xlsx
@@ -2930,10 +2930,6 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" altLang="zh-CN"/>
-                  <a:t>#</a:t>
-                </a:r>
                 <a:r>
                   <a:rPr lang="zh-CN" altLang="en-US" baseline="0"/>
                   <a:t> </a:t>
@@ -4158,8 +4154,8 @@
   <sheetPr/>
   <dimension ref="A1:AZ65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="87" topLeftCell="AB12" workbookViewId="0">
-      <selection activeCell="AD34" sqref="AD34"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="87" topLeftCell="AE12" workbookViewId="0">
+      <selection activeCell="AU15" sqref="AU15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>